<commit_message>
added GSA and PMRA models
</commit_message>
<xml_diff>
--- a/models/Model_summary_statistics.xlsx
+++ b/models/Model_summary_statistics.xlsx
@@ -5,10 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="1000G_FIN_models" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="GSA_models" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="PMRA_models" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="40">
   <si>
     <t xml:space="preserve">Locus</t>
   </si>
@@ -31,7 +33,7 @@
     <t xml:space="preserve">Alleles</t>
   </si>
   <si>
-    <t xml:space="preserve">Train_n</t>
+    <t xml:space="preserve">Samples</t>
   </si>
   <si>
     <t xml:space="preserve">OOB</t>
@@ -61,23 +63,7 @@
     <t xml:space="preserve">II</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">FinnGen ThermoFisher Axiom custom array v2 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">∩ 1000G</t>
-    </r>
+    <t xml:space="preserve">FinnGen ThermoFisher Axiom custom array v2 ∩ 1000G</t>
   </si>
   <si>
     <t xml:space="preserve">III</t>
@@ -138,6 +124,24 @@
   </si>
   <si>
     <t xml:space="preserve">HLA-G_5UTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FinnGen ThermoFisher Axiom custom array v2 ∩ 1000G ∩ Illumina Global Screening Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WES ∩ 1000G ∩ Illumina Global Screening Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FinnGen ThermoFisher Axiom custom array v2 ∩ Illumina Global Screening Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FinnGen ThermoFisher Axiom custom array v2 ∩ 1000G ∩ ThermoFisher Precision Medicine Research Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WES ∩ 1000G ∩ ThermoFisher Precision Medicine Research Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FinnGen ThermoFisher Axiom custom array v2 ∩ ThermoFisher Precision Medicine Research Array</t>
   </si>
 </sst>
 </file>
@@ -150,11 +154,12 @@
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -170,12 +175,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -227,16 +226,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -244,31 +243,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -276,7 +267,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -303,14 +294,14 @@
   </sheetPr>
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N21" activeCellId="0" sqref="N21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.35"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -326,7 +317,7 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
@@ -346,7 +337,7 @@
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5" t="n">
+      <c r="C2" s="4" t="n">
         <v>21</v>
       </c>
       <c r="D2" s="3" t="n">
@@ -369,16 +360,16 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="5" t="n">
+      <c r="C3" s="4" t="n">
         <v>21</v>
       </c>
       <c r="D3" s="3" t="n">
         <v>761</v>
       </c>
-      <c r="E3" s="5" t="n">
+      <c r="E3" s="4" t="n">
         <v>99.3</v>
       </c>
       <c r="F3" s="3" t="n">
@@ -387,7 +378,7 @@
       <c r="G3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -395,16 +386,16 @@
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="5" t="n">
+      <c r="C4" s="4" t="n">
         <v>24</v>
       </c>
       <c r="D4" s="3" t="n">
         <v>327</v>
       </c>
-      <c r="E4" s="5" t="n">
+      <c r="E4" s="4" t="n">
         <v>97.9</v>
       </c>
       <c r="F4" s="3" t="n">
@@ -413,7 +404,7 @@
       <c r="G4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -421,16 +412,16 @@
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="4" t="n">
         <v>27</v>
       </c>
       <c r="D5" s="3" t="n">
         <v>1088</v>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" s="4" t="n">
         <v>99.1</v>
       </c>
       <c r="F5" s="3" t="n">
@@ -439,7 +430,7 @@
       <c r="G5" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -447,16 +438,16 @@
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" s="4" t="n">
         <v>43</v>
       </c>
       <c r="D6" s="3" t="n">
         <v>1555</v>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" s="4" t="n">
         <v>97.6</v>
       </c>
       <c r="F6" s="3" t="n">
@@ -465,7 +456,7 @@
       <c r="G6" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -473,16 +464,16 @@
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="4" t="n">
         <v>45</v>
       </c>
       <c r="D7" s="3" t="n">
         <v>2316</v>
       </c>
-      <c r="E7" s="5" t="n">
+      <c r="E7" s="4" t="n">
         <v>98.2</v>
       </c>
       <c r="F7" s="3" t="n">
@@ -491,7 +482,7 @@
       <c r="G7" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -499,16 +490,16 @@
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="4" t="n">
         <v>43</v>
       </c>
       <c r="D8" s="3" t="n">
         <v>1555</v>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E8" s="4" t="n">
         <v>97.8</v>
       </c>
       <c r="F8" s="3" t="n">
@@ -528,7 +519,7 @@
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" s="4" t="n">
         <v>17</v>
       </c>
       <c r="D9" s="3" t="n">
@@ -551,10 +542,10 @@
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="5" t="n">
+      <c r="C10" s="4" t="n">
         <v>17</v>
       </c>
       <c r="D10" s="3" t="n">
@@ -569,19 +560,19 @@
       <c r="G10" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K10" s="1"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="8"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="6"/>
       <c r="R10" s="1"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
     </row>
@@ -589,10 +580,10 @@
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="5" t="n">
+      <c r="C11" s="4" t="n">
         <v>13</v>
       </c>
       <c r="D11" s="3" t="n">
@@ -607,30 +598,30 @@
       <c r="G11" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K11" s="1"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
       <c r="R11" s="1"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
-      <c r="U11" s="11"/>
-      <c r="V11" s="5"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="5" t="n">
+      <c r="C12" s="4" t="n">
         <v>18</v>
       </c>
       <c r="D12" s="3" t="n">
@@ -645,30 +636,30 @@
       <c r="G12" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K12" s="1"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
       <c r="R12" s="1"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="10"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="5"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="5" t="n">
+      <c r="C13" s="4" t="n">
         <v>19</v>
       </c>
       <c r="D13" s="3" t="n">
@@ -683,30 +674,30 @@
       <c r="G13" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K13" s="1"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
       <c r="R13" s="1"/>
-      <c r="S13" s="12"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="13"/>
-      <c r="V13" s="4"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="5" t="n">
+      <c r="C14" s="4" t="n">
         <v>22</v>
       </c>
       <c r="D14" s="3" t="n">
@@ -721,7 +712,7 @@
       <c r="G14" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -729,10 +720,10 @@
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="5" t="n">
+      <c r="C15" s="4" t="n">
         <v>19</v>
       </c>
       <c r="D15" s="3" t="n">
@@ -758,7 +749,7 @@
       <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="5" t="n">
+      <c r="C16" s="4" t="n">
         <v>4</v>
       </c>
       <c r="D16" s="3" t="n">
@@ -781,16 +772,16 @@
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="5" t="n">
+      <c r="C17" s="4" t="n">
         <v>4</v>
       </c>
       <c r="D17" s="3" t="n">
         <v>441</v>
       </c>
-      <c r="E17" s="5" t="n">
+      <c r="E17" s="4" t="n">
         <v>99.8</v>
       </c>
       <c r="F17" s="3" t="n">
@@ -799,7 +790,7 @@
       <c r="G17" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -807,16 +798,16 @@
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="5" t="n">
+      <c r="C18" s="4" t="n">
         <v>6</v>
       </c>
       <c r="D18" s="3" t="n">
         <v>478</v>
       </c>
-      <c r="E18" s="5" t="n">
+      <c r="E18" s="4" t="n">
         <v>99.6</v>
       </c>
       <c r="F18" s="3" t="n">
@@ -825,7 +816,7 @@
       <c r="G18" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -833,16 +824,16 @@
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="5" t="n">
+      <c r="C19" s="4" t="n">
         <v>6</v>
       </c>
       <c r="D19" s="3" t="n">
         <v>919</v>
       </c>
-      <c r="E19" s="5" t="n">
+      <c r="E19" s="4" t="n">
         <v>99.7</v>
       </c>
       <c r="F19" s="3" t="n">
@@ -851,7 +842,7 @@
       <c r="G19" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -859,16 +850,16 @@
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="5" t="n">
+      <c r="C20" s="4" t="n">
         <v>10</v>
       </c>
       <c r="D20" s="3" t="n">
         <v>2037</v>
       </c>
-      <c r="E20" s="5" t="n">
+      <c r="E20" s="4" t="n">
         <v>99.2</v>
       </c>
       <c r="F20" s="3" t="n">
@@ -877,7 +868,7 @@
       <c r="G20" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -885,16 +876,16 @@
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="5" t="n">
+      <c r="C21" s="4" t="n">
         <v>10</v>
       </c>
       <c r="D21" s="3" t="n">
         <v>2478</v>
       </c>
-      <c r="E21" s="5" t="n">
+      <c r="E21" s="4" t="n">
         <v>99.3</v>
       </c>
       <c r="F21" s="3" t="n">
@@ -903,7 +894,7 @@
       <c r="G21" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -911,16 +902,16 @@
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="5" t="n">
+      <c r="C22" s="4" t="n">
         <v>10</v>
       </c>
       <c r="D22" s="3" t="n">
         <v>2037</v>
       </c>
-      <c r="E22" s="5" t="n">
+      <c r="E22" s="4" t="n">
         <v>99.7</v>
       </c>
       <c r="F22" s="3" t="n">
@@ -940,7 +931,7 @@
       <c r="B23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="5" t="n">
+      <c r="C23" s="4" t="n">
         <v>3</v>
       </c>
       <c r="D23" s="3" t="n">
@@ -963,16 +954,16 @@
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="5" t="n">
+      <c r="C24" s="4" t="n">
         <v>3</v>
       </c>
       <c r="D24" s="3" t="n">
         <v>211</v>
       </c>
-      <c r="E24" s="5" t="n">
+      <c r="E24" s="4" t="n">
         <v>99.9</v>
       </c>
       <c r="F24" s="3" t="n">
@@ -989,16 +980,16 @@
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="5" t="n">
+      <c r="C25" s="4" t="n">
         <v>3</v>
       </c>
       <c r="D25" s="3" t="n">
         <v>296</v>
       </c>
-      <c r="E25" s="5" t="n">
+      <c r="E25" s="4" t="n">
         <v>99.8</v>
       </c>
       <c r="F25" s="3" t="n">
@@ -1007,7 +998,7 @@
       <c r="G25" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="H25" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1015,16 +1006,16 @@
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="5" t="n">
+      <c r="C26" s="4" t="n">
         <v>3</v>
       </c>
       <c r="D26" s="3" t="n">
         <v>507</v>
       </c>
-      <c r="E26" s="5" t="n">
+      <c r="E26" s="4" t="n">
         <v>99.9</v>
       </c>
       <c r="F26" s="3" t="n">
@@ -1033,7 +1024,7 @@
       <c r="G26" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H26" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1041,16 +1032,16 @@
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="5" t="n">
+      <c r="C27" s="4" t="n">
         <v>5</v>
       </c>
       <c r="D27" s="3" t="n">
         <v>1293</v>
       </c>
-      <c r="E27" s="5" t="n">
+      <c r="E27" s="4" t="n">
         <v>99.7</v>
       </c>
       <c r="F27" s="3" t="n">
@@ -1059,7 +1050,7 @@
       <c r="G27" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="H27" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1067,16 +1058,16 @@
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="5" t="n">
+      <c r="C28" s="4" t="n">
         <v>5</v>
       </c>
       <c r="D28" s="3" t="n">
         <v>1504</v>
       </c>
-      <c r="E28" s="5" t="n">
+      <c r="E28" s="4" t="n">
         <v>99.8</v>
       </c>
       <c r="F28" s="3" t="n">
@@ -1085,7 +1076,7 @@
       <c r="G28" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="H28" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1093,16 +1084,16 @@
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="5" t="n">
+      <c r="C29" s="4" t="n">
         <v>5</v>
       </c>
       <c r="D29" s="3" t="n">
         <v>1293</v>
       </c>
-      <c r="E29" s="5" t="n">
+      <c r="E29" s="4" t="n">
         <v>99.9</v>
       </c>
       <c r="F29" s="3" t="n">
@@ -1126,7 +1117,7 @@
         <v>20</v>
       </c>
       <c r="D30" s="3" t="n">
-        <v>296</v>
+        <v>435</v>
       </c>
       <c r="E30" s="3" t="n">
         <v>98.1</v>
@@ -1137,7 +1128,7 @@
       <c r="G30" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="H30" s="6" t="s">
+      <c r="H30" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1152,7 +1143,7 @@
         <v>9</v>
       </c>
       <c r="D31" s="3" t="n">
-        <v>293</v>
+        <v>435</v>
       </c>
       <c r="E31" s="3" t="n">
         <v>99.7</v>
@@ -1163,7 +1154,7 @@
       <c r="G31" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="H31" s="6" t="s">
+      <c r="H31" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1178,7 +1169,7 @@
         <v>10</v>
       </c>
       <c r="D32" s="3" t="n">
-        <v>293</v>
+        <v>435</v>
       </c>
       <c r="E32" s="3" t="n">
         <v>99.4</v>
@@ -1189,7 +1180,7 @@
       <c r="G32" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="H32" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1202,4 +1193,420 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>2316</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>97.6</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1481</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>2367</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>99.1</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1483</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>2478</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>99.4</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1590</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1504</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>99.8</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1305</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>435</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>98.4</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1093</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>435</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>99.7</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>671</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>435</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>99.4</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1001</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>2316</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>97.6</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1168</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>2367</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>98.9</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1234</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>2478</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>99.2</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1283</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1504</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>99.8</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1327</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>435</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>98.5</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1080</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>435</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>99.7</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>674</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>435</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>99.3</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>979</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>